<commit_message>
Updated theme_track_config to match new parser
</commit_message>
<xml_diff>
--- a/theme_track_config.xlsx
+++ b/theme_track_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="112">
   <si>
     <t xml:space="preserve">Options</t>
   </si>
@@ -29,13 +29,281 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Report Currency</t>
+    <t xml:space="preserve">ReportCurrency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Native report currency. All currencies will be converted to this when displayed on reports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ThemeReport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capex Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AlwaysShowPicks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CapGains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categories of this pick type always show in table, regardless if there are funds allocated to it or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skeleton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display As</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel Format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columns to display. Column names are in ‘Joined Data’ sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:CurrValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invested in Theme ${ReportCurrency}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CurrencyFormat}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:CatTotalPerc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of Total Invested in Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SecuritiesReport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capex Stocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:CapexGainsPickTypeShortDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portofolio(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Exchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Ticker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value ${ReportCurrency}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:CatPerc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:TotalPerc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divi Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divi Stocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CurrencyFormat</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">How each currency is displayed. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Can be used above in any field as the “Excel Format”, by specifying “${CurrencyFormat}"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExcelFormat</t>
   </si>
   <si>
     <t xml:space="preserve">USD</t>
   </si>
   <si>
-    <t xml:space="preserve">Native report currency. All currencies will be converted to this when displayed on reports</t>
+    <t xml:space="preserve">"$"#,##0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"€"#,##0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"£"#,##0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">British Pound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"¥"#,##0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japanese Yen (no decimal places)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"¥"#,##0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinese Yuan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"₹"#,##0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indian Rupee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australian Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canadian Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"CHF"#,##0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swiss Franc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HKD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hong Kong Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NZD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Zealand Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KRW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"₩"#,##0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Korean Won (no decimal places)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SGD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singapore Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"R$"#,##0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazilian Real</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"R"#,##0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South African Rand</t>
   </si>
   <si>
     <t xml:space="preserve">Rules are processed in order</t>
@@ -74,9 +342,6 @@
     <t xml:space="preserve">InteractiveBrokers</t>
   </si>
   <si>
-    <t xml:space="preserve">R:Exchange</t>
-  </si>
-  <si>
     <t xml:space="preserve">HK</t>
   </si>
   <si>
@@ -87,9 +352,6 @@
   </si>
   <si>
     <t xml:space="preserve">PINK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:Ticker</t>
   </si>
   <si>
     <t xml:space="preserve">Symbol</t>
@@ -117,11 +379,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -149,6 +412,18 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -193,8 +468,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -202,11 +481,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -227,55 +514,675 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:AMJ65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="5" style="1" width="11.63"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2"/>
+      <c r="B34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="6"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F10" r:id="rId1" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F19" r:id="rId2" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F32" r:id="rId3" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F40" r:id="rId4" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -293,11 +1200,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
@@ -307,92 +1214,92 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+    <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
+    <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
+    <row r="5" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
+    <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1" t="s">
+    <row r="9" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="AMJ9" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2343</v>
@@ -400,38 +1307,38 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1171</v>
@@ -439,38 +1346,38 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>25</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now report columns should be configurable
</commit_message>
<xml_diff>
--- a/theme_track_config.xlsx
+++ b/theme_track_config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="114">
   <si>
     <t xml:space="preserve">Options</t>
   </si>
@@ -95,7 +95,7 @@
     <t xml:space="preserve">${CurrencyFormat}</t>
   </si>
   <si>
-    <t xml:space="preserve">R:CatTotalPerc</t>
+    <t xml:space="preserve">R:TotalPerc</t>
   </si>
   <si>
     <t xml:space="preserve">% of Total Invested in Theme</t>
@@ -104,6 +104,9 @@
     <t xml:space="preserve">0.00%</t>
   </si>
   <si>
+    <t xml:space="preserve">ColumnOrder</t>
+  </si>
+  <si>
     <t xml:space="preserve">SecuritiesReport</t>
   </si>
   <si>
@@ -137,12 +140,12 @@
     <t xml:space="preserve">% of Theme</t>
   </si>
   <si>
-    <t xml:space="preserve">R:TotalPerc</t>
-  </si>
-  <si>
     <t xml:space="preserve">% of Total</t>
   </si>
   <si>
+    <t xml:space="preserve">D:CapexGainsPickTypeOrder</t>
+  </si>
+  <si>
     <t xml:space="preserve">Divi Theme</t>
   </si>
   <si>
@@ -158,26 +161,13 @@
     <t xml:space="preserve">Divi Stocks</t>
   </si>
   <si>
+    <t xml:space="preserve">D:DiviPickTypeOrder</t>
+  </si>
+  <si>
     <t xml:space="preserve">CurrencyFormat</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">How each currency is displayed. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Can be used above in any field as the “Excel Format”, by specifying “${CurrencyFormat}"</t>
-    </r>
+    <t xml:space="preserve">How each currency is displayed. Can be used above in any field as the “Excel Format”, by specifying “${CurrencyFormat}"</t>
   </si>
   <si>
     <t xml:space="preserve">Types</t>
@@ -384,7 +374,7 @@
     <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -419,11 +409,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -514,10 +499,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ65"/>
+  <dimension ref="A1:AMJ87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -643,230 +628,198 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="1" t="s">
-        <v>17</v>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>19</v>
+      <c r="A22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="B31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2"/>
-      <c r="B34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,314 +827,459 @@
         <v>6</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="1" t="s">
+      <c r="E40" s="2"/>
+      <c r="F40" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="F41" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2"/>
       <c r="B43" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="B44" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="2"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F50" s="0"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B53" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B54" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="A55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="2"/>
       <c r="F55" s="1" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>66</v>
+        <v>42</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>68</v>
+        <v>30</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>70</v>
+        <v>32</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>73</v>
+        <v>34</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>75</v>
+        <v>21</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E61" s="5"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="B63" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="6"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="6"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="6"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F72" s="0"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F65" s="1" t="s">
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="1" t="s">
         <v>88</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
-    <hyperlink ref="F19" r:id="rId2" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
-    <hyperlink ref="F32" r:id="rId3" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
-    <hyperlink ref="F40" r:id="rId4" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F23" r:id="rId2" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F41" r:id="rId3" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F56" r:id="rId4" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1201,10 +1299,10 @@
   <dimension ref="A1:AMJ20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B43 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
@@ -1216,7 +1314,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -1225,28 +1323,28 @@
     </row>
     <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AMJ5" s="0"/>
     </row>
@@ -1255,7 +1353,7 @@
     </row>
     <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="AMJ7" s="0"/>
     </row>
@@ -1264,10 +1362,10 @@
     </row>
     <row r="9" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>1</v>
@@ -1276,30 +1374,30 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2343</v>
@@ -1307,38 +1405,38 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1171</v>
@@ -1346,38 +1444,38 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now forex will read from the web during snapshot creation reports now have total, and also fixed theme reports
</commit_message>
<xml_diff>
--- a/theme_track_config.xlsx
+++ b/theme_track_config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="115">
   <si>
     <t xml:space="preserve">Options</t>
   </si>
@@ -32,160 +32,163 @@
     <t xml:space="preserve">ReportCurrency</t>
   </si>
   <si>
+    <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Native report currency. All currencies will be converted to this when displayed on reports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ThemeReport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capex Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AlwaysShowPicks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CapGains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categories of this pick type always show in table, regardless if there are funds allocated to it or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skeleton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display As</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel Format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columns to display. Column names are in ‘Joined Data’ sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:CurrValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invested in Theme ${ReportCurrency}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CurrencyFormat}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:TotalPerc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of Total Invested in Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ColumnOrder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SumColumns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SecuritiesReport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capex Stocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:CapexGainsPickTypeShortDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portofolio(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Exchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Ticker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value ${ReportCurrency}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:CatPerc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:CapexGainsPickTypeOrder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divi Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divi Stocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:DiviPickTypeOrder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CurrencyFormat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How each currency is displayed. Can be used above in any field as the “Excel Format”, by specifying “${CurrencyFormat}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExcelFormat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"$"#,##0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Dollar</t>
+  </si>
+  <si>
     <t xml:space="preserve">EUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Native report currency. All currencies will be converted to this when displayed on reports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeReport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capex Theme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:Theme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AlwaysShowPicks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CapGains</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categories of this pick type always show in table, regardless if there are funds allocated to it or not</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skeleton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Columns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display As</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excel Format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Columns to display. Column names are in ‘Joined Data’ sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Theme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:CurrValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invested in Theme ${ReportCurrency}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CurrencyFormat}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:TotalPerc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of Total Invested in Theme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColumnOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SecuritiesReport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capex Stocks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D:CapexGainsPickTypeShortDesc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portofolio(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:Exchange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exchange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:Ticker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ticker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value ${ReportCurrency}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:CatPerc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of Theme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D:CapexGainsPickTypeOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divi Theme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:Sector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divi Stocks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D:DiviPickTypeOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CurrencyFormat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How each currency is displayed. Can be used above in any field as the “Excel Format”, by specifying “${CurrencyFormat}"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ExcelFormat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"$"#,##0.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US Dollar</t>
   </si>
   <si>
     <t xml:space="preserve">"€"#,##0.00</t>
@@ -499,10 +502,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ87"/>
+  <dimension ref="A1:AMJ89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -636,9 +639,22 @@
         <v>9</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,7 +662,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,10 +724,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>19</v>
@@ -719,10 +735,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>19</v>
@@ -730,10 +746,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>19</v>
@@ -744,7 +760,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>23</v>
@@ -752,10 +768,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>26</v>
@@ -767,7 +783,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>26</v>
@@ -787,7 +803,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="5"/>
@@ -795,7 +811,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="5"/>
@@ -803,220 +819,230 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C34" s="3"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2"/>
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="1" t="s">
+      <c r="E42" s="2"/>
+      <c r="F42" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41" s="1" t="s">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="1" t="s">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2"/>
-      <c r="B43" s="1" t="s">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2"/>
+      <c r="B45" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D45" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
+      <c r="B46" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="B48" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="A51" s="2"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="1" t="s">
+      <c r="E57" s="2"/>
+      <c r="F57" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="F58" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>19</v>
@@ -1024,262 +1050,291 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E61" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D63" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E62" s="5"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="B65" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="1" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="6"/>
+      <c r="B67" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="6"/>
+      <c r="B68" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="6"/>
+      <c r="A69" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F71" s="0" t="s">
+      <c r="B71" s="6"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="s">
+      <c r="F73" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B72" s="2" t="s">
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F72" s="0"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="1" t="s">
+      <c r="C74" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="F74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="1" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C87" s="1" t="s">
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F87" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>90</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
     <hyperlink ref="F23" r:id="rId2" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
-    <hyperlink ref="F41" r:id="rId3" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
-    <hyperlink ref="F56" r:id="rId4" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F43" r:id="rId3" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
+    <hyperlink ref="F58" r:id="rId4" display="Excel Formats are according to https://support.microsoft.com/en-us/office/number-format-codes-5026bbd6-04bc-48cd-bf33-80f18b4eae68"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1299,10 +1354,10 @@
   <dimension ref="A1:AMJ20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B43 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
@@ -1314,7 +1369,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -1323,28 +1378,28 @@
     </row>
     <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AMJ5" s="0"/>
     </row>
@@ -1353,7 +1408,7 @@
     </row>
     <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AMJ7" s="0"/>
     </row>
@@ -1362,10 +1417,10 @@
     </row>
     <row r="9" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>1</v>
@@ -1374,30 +1429,30 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2343</v>
@@ -1405,38 +1460,38 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1171</v>
@@ -1444,38 +1499,38 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
about to try and add transaction, rate of return, etc.
</commit_message>
<xml_diff>
--- a/theme_track_config.xlsx
+++ b/theme_track_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="116">
   <si>
     <t xml:space="preserve">Options</t>
   </si>
@@ -505,10 +505,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ90"/>
+  <dimension ref="A1:AMJ91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="A22:C22 B30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="66:66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1121,226 +1121,238 @@
       <c r="E65" s="5"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="s">
+      <c r="B66" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="s">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="1" t="s">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="6"/>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F74" s="0" t="s">
-        <v>50</v>
-      </c>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F75" s="0"/>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="F76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F90" s="1" t="s">
+      <c r="F91" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1368,8 +1380,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22:C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="1" sqref="66:66 A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>